<commit_message>
update reapro with new template
</commit_message>
<xml_diff>
--- a/client/public/templates/Stock Data.xlsx
+++ b/client/public/templates/Stock Data.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27618"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9255FC29-3A82-4BDB-A3D5-9190A21ED4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72B53421-F3A3-4422-A512-5BB4FBFC0373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,8 +30,108 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={F822D681-0EAE-4E9B-A455-EBB00BC11D69}</author>
+    <author>tc={420E1286-AF6C-4897-BC09-D76D56B716BB}</author>
+    <author>tc={55EBDCFF-9B44-4D91-B08E-88AC7C6BEEB4}</author>
+    <author>tc={850B46C8-7988-43E4-8D59-C028C1E1A9CF}</author>
+    <author>tc={1863AC7F-0513-48A0-8A84-D688EFE67609}</author>
+    <author>tc={8064FE14-C340-4A51-A672-5E6C0C3B25DF}</author>
+    <author>tc={7EA48935-1464-445E-8D3F-2C95EAFA1621}</author>
+    <author>tc={DDCAD24E-4B91-44F7-A0C2-B7C9FF4BFA6C}</author>
+    <author>tc={E1EBB7E0-1C19-4A72-BDD6-27D7771C580F}</author>
+  </authors>
+  <commentList>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{F822D681-0EAE-4E9B-A455-EBB00BC11D69}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Stock fisico</t>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="1" shapeId="0" xr:uid="{420E1286-AF6C-4897-BC09-D76D56B716BB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Ordenes de venta pendientes de entregar</t>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="2" shapeId="0" xr:uid="{55EBDCFF-9B44-4D91-B08E-88AC7C6BEEB4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tiempo de entrega de proveedor</t>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="3" shapeId="0" xr:uid="{850B46C8-7988-43E4-8D59-C028C1E1A9CF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Lote optimo de compra a partir del costo del inventario y del costo de la compra</t>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="4" shapeId="0" xr:uid="{1863AC7F-0513-48A0-8A84-D688EFE67609}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Nivel de Servicio 
+97 - 99 para productos A
+95 - 98 para productos B
+90 - 95 para productos C</t>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="5" shapeId="0" xr:uid="{8064FE14-C340-4A51-A672-5E6C0C3B25DF}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Nivel de certeza del proveedor 
+Días demorados de los pedidos tradicionales
+Ejemplo: Si normalmente demora 15 días, pero a veces demora 40 días, este parametro seria:
+Lead time = 15
+Desv Est Lt Days = 25</t>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="6" shapeId="0" xr:uid="{7EA48935-1464-445E-8D3F-2C95EAFA1621}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Ordenes de compra pendiente de ingreso</t>
+      </text>
+    </comment>
+    <comment ref="T1" authorId="7" shapeId="0" xr:uid="{DDCAD24E-4B91-44F7-A0C2-B7C9FF4BFA6C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ABC segun Pareto 
+A = Item 80% de la venta
+B = Item 15% de la venta
+C = Item 5% de la venta</t>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="8" shapeId="0" xr:uid="{E1EBB7E0-1C19-4A72-BDD6-27D7771C580F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Categorización del producto segun lo estrategico del mismo</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Family</t>
   </si>
@@ -57,16 +157,16 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Available Stock</t>
-  </si>
-  <si>
-    <t>Pending Stock</t>
-  </si>
-  <si>
-    <t>Safety Lead Time</t>
-  </si>
-  <si>
-    <t>Safety stock</t>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Sales Order Pending Deliverys</t>
+  </si>
+  <si>
+    <t>Safety Lead Time (days)</t>
+  </si>
+  <si>
+    <t>Safety stock (days)</t>
   </si>
   <si>
     <t>Lead Time</t>
@@ -75,7 +175,7 @@
     <t>Price</t>
   </si>
   <si>
-    <t>Optimal Batch</t>
+    <t>EOQ (Economical order quantity)</t>
   </si>
   <si>
     <t>Service Level</t>
@@ -88,6 +188,12 @@
   </si>
   <si>
     <t>Lot Sizing</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -199,6 +305,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="GARCIA , MATIAS NICOLAS" id="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" userId="S::garciamatias159@ies21.onmicrosoft.com::0ed3d248-6599-4c4c-b5bc-25771ec13e7d" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -516,12 +628,54 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="I1" dT="2024-04-23T18:11:08.09" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{F822D681-0EAE-4E9B-A455-EBB00BC11D69}">
+    <text>Stock fisico</text>
+  </threadedComment>
+  <threadedComment ref="J1" dT="2024-04-23T18:09:32.08" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{420E1286-AF6C-4897-BC09-D76D56B716BB}">
+    <text>Ordenes de venta pendientes de entregar</text>
+  </threadedComment>
+  <threadedComment ref="M1" dT="2024-04-23T18:12:43.18" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{55EBDCFF-9B44-4D91-B08E-88AC7C6BEEB4}">
+    <text>Tiempo de entrega de proveedor</text>
+  </threadedComment>
+  <threadedComment ref="O1" dT="2024-04-23T18:15:20.09" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{850B46C8-7988-43E4-8D59-C028C1E1A9CF}">
+    <text>Lote optimo de compra a partir del costo del inventario y del costo de la compra</text>
+  </threadedComment>
+  <threadedComment ref="P1" dT="2024-04-23T18:15:32.86" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{1863AC7F-0513-48A0-8A84-D688EFE67609}">
+    <text>Nivel de Servicio 
+97 - 99 para productos A
+95 - 98 para productos B
+90 - 95 para productos C</text>
+  </threadedComment>
+  <threadedComment ref="Q1" dT="2024-04-23T18:18:05.68" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{8064FE14-C340-4A51-A672-5E6C0C3B25DF}">
+    <text>Nivel de certeza del proveedor 
+Días demorados de los pedidos tradicionales
+Ejemplo: Si normalmente demora 15 días, pero a veces demora 40 días, este parametro seria:
+Lead time = 15
+Desv Est Lt Days = 25</text>
+  </threadedComment>
+  <threadedComment ref="R1" dT="2024-04-23T18:18:30.37" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{7EA48935-1464-445E-8D3F-2C95EAFA1621}">
+    <text>Ordenes de compra pendiente de ingreso</text>
+  </threadedComment>
+  <threadedComment ref="T1" dT="2024-04-23T18:19:24.23" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{DDCAD24E-4B91-44F7-A0C2-B7C9FF4BFA6C}">
+    <text>ABC segun Pareto 
+A = Item 80% de la venta
+B = Item 15% de la venta
+C = Item 5% de la venta</text>
+  </threadedComment>
+  <threadedComment ref="U1" dT="2024-04-23T18:21:06.92" personId="{C7861E8F-5ED8-47F7-8704-334A9BFE4329}" id="{E1EBB7E0-1C19-4A72-BDD6-27D7771C580F}">
+    <text>Categorización del producto segun lo estrategico del mismo</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -535,12 +689,12 @@
     <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
     <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -603,9 +757,13 @@
       <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
       <c r="Y1" s="3"/>
@@ -623,5 +781,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>